<commit_message>
add -- update security config
</commit_message>
<xml_diff>
--- a/uploads/template-d9.xlsx
+++ b/uploads/template-d9.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27852" uniqueCount="331">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28572" uniqueCount="331">
   <si>
     <t>Description</t>
   </si>
@@ -1290,7 +1290,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="100">
+  <cellXfs count="102">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -1320,6 +1320,13 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="true">
+      <alignment wrapText="true"/>
+      <protection locked="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="true">
+      <protection locked="false"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="true">
       <alignment wrapText="true"/>
@@ -1935,2402 +1942,2402 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="98" t="s">
+      <c r="A2" s="100" t="s">
         <v>180</v>
       </c>
-      <c r="B2" s="98" t="s">
+      <c r="B2" s="100" t="s">
         <v>140</v>
       </c>
-      <c r="C2" s="98" t="s">
+      <c r="C2" s="100" t="s">
         <v>182</v>
       </c>
-      <c r="D2" s="98" t="s">
+      <c r="D2" s="100" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="99" t="s">
-        <v>141</v>
-      </c>
-      <c r="F2" s="99" t="s">
+      <c r="E2" s="101" t="s">
+        <v>141</v>
+      </c>
+      <c r="F2" s="101" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="98" t="s">
+      <c r="A3" s="100" t="s">
         <v>180</v>
       </c>
-      <c r="B3" s="98" t="s">
+      <c r="B3" s="100" t="s">
         <v>140</v>
       </c>
-      <c r="C3" s="98" t="s">
+      <c r="C3" s="100" t="s">
         <v>180</v>
       </c>
-      <c r="D3" s="98" t="s">
+      <c r="D3" s="100" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="99" t="s">
-        <v>141</v>
-      </c>
-      <c r="F3" s="99" t="s">
+      <c r="E3" s="101" t="s">
+        <v>141</v>
+      </c>
+      <c r="F3" s="101" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="98" t="s">
+      <c r="A4" s="100" t="s">
         <v>180</v>
       </c>
-      <c r="B4" s="98" t="s">
+      <c r="B4" s="100" t="s">
         <v>140</v>
       </c>
-      <c r="C4" s="98" t="s">
+      <c r="C4" s="100" t="s">
         <v>181</v>
       </c>
-      <c r="D4" s="98" t="s">
+      <c r="D4" s="100" t="s">
         <v>300</v>
       </c>
-      <c r="E4" s="99" t="s">
-        <v>141</v>
-      </c>
-      <c r="F4" s="99" t="s">
+      <c r="E4" s="101" t="s">
+        <v>141</v>
+      </c>
+      <c r="F4" s="101" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="98" t="s">
+      <c r="A5" s="100" t="s">
         <v>180</v>
       </c>
-      <c r="B5" s="98" t="s">
+      <c r="B5" s="100" t="s">
         <v>140</v>
       </c>
-      <c r="C5" s="98" t="s">
+      <c r="C5" s="100" t="s">
         <v>185</v>
       </c>
-      <c r="D5" s="98" t="s">
+      <c r="D5" s="100" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="99" t="s">
-        <v>141</v>
-      </c>
-      <c r="F5" s="99" t="s">
+      <c r="E5" s="101" t="s">
+        <v>141</v>
+      </c>
+      <c r="F5" s="101" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="98" t="s">
+      <c r="A6" s="100" t="s">
         <v>180</v>
       </c>
-      <c r="B6" s="98" t="s">
+      <c r="B6" s="100" t="s">
         <v>140</v>
       </c>
-      <c r="C6" s="98" t="s">
+      <c r="C6" s="100" t="s">
         <v>184</v>
       </c>
-      <c r="D6" s="98" t="s">
+      <c r="D6" s="100" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="99" t="s">
-        <v>141</v>
-      </c>
-      <c r="F6" s="99" t="s">
+      <c r="E6" s="101" t="s">
+        <v>141</v>
+      </c>
+      <c r="F6" s="101" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="98" t="s">
+      <c r="A7" s="100" t="s">
         <v>180</v>
       </c>
-      <c r="B7" s="98" t="s">
+      <c r="B7" s="100" t="s">
         <v>140</v>
       </c>
-      <c r="C7" s="98" t="s">
+      <c r="C7" s="100" t="s">
         <v>183</v>
       </c>
-      <c r="D7" s="98" t="s">
+      <c r="D7" s="100" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="99" t="s">
-        <v>141</v>
-      </c>
-      <c r="F7" s="99" t="s">
+      <c r="E7" s="101" t="s">
+        <v>141</v>
+      </c>
+      <c r="F7" s="101" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="98" t="s">
+      <c r="A8" s="100" t="s">
         <v>180</v>
       </c>
-      <c r="B8" s="98" t="s">
+      <c r="B8" s="100" t="s">
         <v>140</v>
       </c>
-      <c r="C8" s="98" t="s">
+      <c r="C8" s="100" t="s">
         <v>186</v>
       </c>
-      <c r="D8" s="98" t="s">
+      <c r="D8" s="100" t="s">
         <v>6</v>
       </c>
-      <c r="E8" s="99" t="s">
-        <v>141</v>
-      </c>
-      <c r="F8" s="99" t="s">
+      <c r="E8" s="101" t="s">
+        <v>141</v>
+      </c>
+      <c r="F8" s="101" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="98" t="s">
+      <c r="A9" s="100" t="s">
         <v>182</v>
       </c>
-      <c r="B9" s="98" t="s">
+      <c r="B9" s="100" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="98" t="s">
+      <c r="C9" s="100" t="s">
         <v>193</v>
       </c>
-      <c r="D9" s="98" t="s">
+      <c r="D9" s="100" t="s">
         <v>22</v>
       </c>
-      <c r="E9" s="99" t="s">
-        <v>141</v>
-      </c>
-      <c r="F9" s="99" t="s">
+      <c r="E9" s="101" t="s">
+        <v>141</v>
+      </c>
+      <c r="F9" s="101" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="98" t="s">
+      <c r="A10" s="100" t="s">
         <v>182</v>
       </c>
-      <c r="B10" s="98" t="s">
+      <c r="B10" s="100" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="98" t="s">
+      <c r="C10" s="100" t="s">
         <v>192</v>
       </c>
-      <c r="D10" s="98" t="s">
+      <c r="D10" s="100" t="s">
         <v>25</v>
       </c>
-      <c r="E10" s="99" t="s">
-        <v>141</v>
-      </c>
-      <c r="F10" s="99" t="s">
+      <c r="E10" s="101" t="s">
+        <v>141</v>
+      </c>
+      <c r="F10" s="101" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="98" t="s">
+      <c r="A11" s="100" t="s">
         <v>182</v>
       </c>
-      <c r="B11" s="98" t="s">
+      <c r="B11" s="100" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="98" t="s">
+      <c r="C11" s="100" t="s">
         <v>197</v>
       </c>
-      <c r="D11" s="98" t="s">
+      <c r="D11" s="100" t="s">
         <v>301</v>
       </c>
-      <c r="E11" s="99" t="s">
-        <v>141</v>
-      </c>
-      <c r="F11" s="99" t="s">
+      <c r="E11" s="101" t="s">
+        <v>141</v>
+      </c>
+      <c r="F11" s="101" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="98" t="s">
+      <c r="A12" s="100" t="s">
         <v>182</v>
       </c>
-      <c r="B12" s="98" t="s">
+      <c r="B12" s="100" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="98" t="s">
+      <c r="C12" s="100" t="s">
         <v>194</v>
       </c>
-      <c r="D12" s="98" t="s">
+      <c r="D12" s="100" t="s">
         <v>26</v>
       </c>
-      <c r="E12" s="99" t="s">
-        <v>141</v>
-      </c>
-      <c r="F12" s="99" t="s">
+      <c r="E12" s="101" t="s">
+        <v>141</v>
+      </c>
+      <c r="F12" s="101" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="98" t="s">
+      <c r="A13" s="100" t="s">
         <v>182</v>
       </c>
-      <c r="B13" s="98" t="s">
+      <c r="B13" s="100" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="98" t="s">
+      <c r="C13" s="100" t="s">
         <v>195</v>
       </c>
-      <c r="D13" s="98" t="s">
+      <c r="D13" s="100" t="s">
         <v>27</v>
       </c>
-      <c r="E13" s="99" t="s">
-        <v>141</v>
-      </c>
-      <c r="F13" s="99" t="s">
+      <c r="E13" s="101" t="s">
+        <v>141</v>
+      </c>
+      <c r="F13" s="101" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="98" t="s">
+      <c r="A14" s="100" t="s">
         <v>182</v>
       </c>
-      <c r="B14" s="98" t="s">
+      <c r="B14" s="100" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="98" t="s">
+      <c r="C14" s="100" t="s">
         <v>188</v>
       </c>
-      <c r="D14" s="98" t="s">
+      <c r="D14" s="100" t="s">
         <v>302</v>
       </c>
-      <c r="E14" s="99" t="s">
-        <v>141</v>
-      </c>
-      <c r="F14" s="99" t="s">
+      <c r="E14" s="101" t="s">
+        <v>141</v>
+      </c>
+      <c r="F14" s="101" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="98" t="s">
+      <c r="A15" s="100" t="s">
         <v>182</v>
       </c>
-      <c r="B15" s="98" t="s">
+      <c r="B15" s="100" t="s">
         <v>11</v>
       </c>
-      <c r="C15" s="98" t="s">
+      <c r="C15" s="100" t="s">
         <v>190</v>
       </c>
-      <c r="D15" s="98" t="s">
+      <c r="D15" s="100" t="s">
         <v>20</v>
       </c>
-      <c r="E15" s="99" t="s">
-        <v>141</v>
-      </c>
-      <c r="F15" s="99" t="s">
+      <c r="E15" s="101" t="s">
+        <v>141</v>
+      </c>
+      <c r="F15" s="101" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="98" t="s">
+      <c r="A16" s="100" t="s">
         <v>182</v>
       </c>
-      <c r="B16" s="98" t="s">
+      <c r="B16" s="100" t="s">
         <v>11</v>
       </c>
-      <c r="C16" s="98" t="s">
+      <c r="C16" s="100" t="s">
         <v>196</v>
       </c>
-      <c r="D16" s="98" t="s">
+      <c r="D16" s="100" t="s">
         <v>303</v>
       </c>
-      <c r="E16" s="99" t="s">
-        <v>141</v>
-      </c>
-      <c r="F16" s="99" t="s">
+      <c r="E16" s="101" t="s">
+        <v>141</v>
+      </c>
+      <c r="F16" s="101" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="98" t="s">
+      <c r="A17" s="100" t="s">
         <v>182</v>
       </c>
-      <c r="B17" s="98" t="s">
+      <c r="B17" s="100" t="s">
         <v>11</v>
       </c>
-      <c r="C17" s="98" t="s">
+      <c r="C17" s="100" t="s">
         <v>187</v>
       </c>
-      <c r="D17" s="98" t="s">
+      <c r="D17" s="100" t="s">
         <v>304</v>
       </c>
-      <c r="E17" s="99" t="s">
-        <v>141</v>
-      </c>
-      <c r="F17" s="99" t="s">
+      <c r="E17" s="101" t="s">
+        <v>141</v>
+      </c>
+      <c r="F17" s="101" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="98" t="s">
+      <c r="A18" s="100" t="s">
         <v>182</v>
       </c>
-      <c r="B18" s="98" t="s">
+      <c r="B18" s="100" t="s">
         <v>11</v>
       </c>
-      <c r="C18" s="98" t="s">
+      <c r="C18" s="100" t="s">
         <v>199</v>
       </c>
-      <c r="D18" s="98" t="s">
+      <c r="D18" s="100" t="s">
         <v>305</v>
       </c>
-      <c r="E18" s="99" t="s">
-        <v>141</v>
-      </c>
-      <c r="F18" s="99" t="s">
+      <c r="E18" s="101" t="s">
+        <v>141</v>
+      </c>
+      <c r="F18" s="101" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="98" t="s">
+      <c r="A19" s="100" t="s">
         <v>182</v>
       </c>
-      <c r="B19" s="98" t="s">
+      <c r="B19" s="100" t="s">
         <v>11</v>
       </c>
-      <c r="C19" s="98" t="s">
+      <c r="C19" s="100" t="s">
         <v>189</v>
       </c>
-      <c r="D19" s="98" t="s">
+      <c r="D19" s="100" t="s">
         <v>306</v>
       </c>
-      <c r="E19" s="99" t="s">
-        <v>141</v>
-      </c>
-      <c r="F19" s="99" t="s">
+      <c r="E19" s="101" t="s">
+        <v>141</v>
+      </c>
+      <c r="F19" s="101" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="98" t="s">
+      <c r="A20" s="100" t="s">
         <v>182</v>
       </c>
-      <c r="B20" s="98" t="s">
+      <c r="B20" s="100" t="s">
         <v>11</v>
       </c>
-      <c r="C20" s="98" t="s">
+      <c r="C20" s="100" t="s">
         <v>191</v>
       </c>
-      <c r="D20" s="98" t="s">
+      <c r="D20" s="100" t="s">
         <v>307</v>
       </c>
-      <c r="E20" s="99" t="s">
-        <v>141</v>
-      </c>
-      <c r="F20" s="99" t="s">
+      <c r="E20" s="101" t="s">
+        <v>141</v>
+      </c>
+      <c r="F20" s="101" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="98" t="s">
+      <c r="A21" s="100" t="s">
         <v>182</v>
       </c>
-      <c r="B21" s="98" t="s">
+      <c r="B21" s="100" t="s">
         <v>11</v>
       </c>
-      <c r="C21" s="98" t="s">
+      <c r="C21" s="100" t="s">
         <v>200</v>
       </c>
-      <c r="D21" s="98" t="s">
+      <c r="D21" s="100" t="s">
         <v>308</v>
       </c>
-      <c r="E21" s="99" t="s">
-        <v>141</v>
-      </c>
-      <c r="F21" s="99" t="s">
+      <c r="E21" s="101" t="s">
+        <v>141</v>
+      </c>
+      <c r="F21" s="101" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="98" t="s">
+      <c r="A22" s="100" t="s">
         <v>182</v>
       </c>
-      <c r="B22" s="98" t="s">
+      <c r="B22" s="100" t="s">
         <v>11</v>
       </c>
-      <c r="C22" s="98" t="s">
+      <c r="C22" s="100" t="s">
         <v>198</v>
       </c>
-      <c r="D22" s="98" t="s">
+      <c r="D22" s="100" t="s">
         <v>309</v>
       </c>
-      <c r="E22" s="99" t="s">
-        <v>141</v>
-      </c>
-      <c r="F22" s="99" t="s">
+      <c r="E22" s="101" t="s">
+        <v>141</v>
+      </c>
+      <c r="F22" s="101" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="98" t="s">
+      <c r="A23" s="100" t="s">
         <v>183</v>
       </c>
-      <c r="B23" s="98" t="s">
+      <c r="B23" s="100" t="s">
         <v>28</v>
       </c>
-      <c r="C23" s="98" t="s">
+      <c r="C23" s="100" t="s">
         <v>201</v>
       </c>
-      <c r="D23" s="98" t="s">
+      <c r="D23" s="100" t="s">
         <v>310</v>
       </c>
-      <c r="E23" s="99" t="s">
-        <v>141</v>
-      </c>
-      <c r="F23" s="99" t="s">
+      <c r="E23" s="101" t="s">
+        <v>141</v>
+      </c>
+      <c r="F23" s="101" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="98" t="s">
+      <c r="A24" s="100" t="s">
         <v>184</v>
       </c>
-      <c r="B24" s="98" t="s">
+      <c r="B24" s="100" t="s">
         <v>147</v>
       </c>
-      <c r="C24" s="98" t="s">
+      <c r="C24" s="100" t="s">
         <v>208</v>
       </c>
-      <c r="D24" s="98" t="s">
+      <c r="D24" s="100" t="s">
         <v>48</v>
       </c>
-      <c r="E24" s="99" t="s">
-        <v>141</v>
-      </c>
-      <c r="F24" s="99" t="s">
+      <c r="E24" s="101" t="s">
+        <v>141</v>
+      </c>
+      <c r="F24" s="101" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="98" t="s">
+      <c r="A25" s="100" t="s">
         <v>184</v>
       </c>
-      <c r="B25" s="98" t="s">
+      <c r="B25" s="100" t="s">
         <v>147</v>
       </c>
-      <c r="C25" s="98" t="s">
+      <c r="C25" s="100" t="s">
         <v>206</v>
       </c>
-      <c r="D25" s="98" t="s">
+      <c r="D25" s="100" t="s">
         <v>45</v>
       </c>
-      <c r="E25" s="99" t="s">
-        <v>141</v>
-      </c>
-      <c r="F25" s="99" t="s">
+      <c r="E25" s="101" t="s">
+        <v>141</v>
+      </c>
+      <c r="F25" s="101" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="98" t="s">
+      <c r="A26" s="100" t="s">
         <v>184</v>
       </c>
-      <c r="B26" s="98" t="s">
+      <c r="B26" s="100" t="s">
         <v>147</v>
       </c>
-      <c r="C26" s="98" t="s">
+      <c r="C26" s="100" t="s">
         <v>202</v>
       </c>
-      <c r="D26" s="98" t="s">
+      <c r="D26" s="100" t="s">
         <v>311</v>
       </c>
-      <c r="E26" s="99" t="s">
-        <v>141</v>
-      </c>
-      <c r="F26" s="99" t="s">
+      <c r="E26" s="101" t="s">
+        <v>141</v>
+      </c>
+      <c r="F26" s="101" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="98" t="s">
+      <c r="A27" s="100" t="s">
         <v>184</v>
       </c>
-      <c r="B27" s="98" t="s">
+      <c r="B27" s="100" t="s">
         <v>147</v>
       </c>
-      <c r="C27" s="98" t="s">
+      <c r="C27" s="100" t="s">
         <v>205</v>
       </c>
-      <c r="D27" s="98" t="s">
+      <c r="D27" s="100" t="s">
         <v>44</v>
       </c>
-      <c r="E27" s="99" t="s">
-        <v>141</v>
-      </c>
-      <c r="F27" s="99" t="s">
+      <c r="E27" s="101" t="s">
+        <v>141</v>
+      </c>
+      <c r="F27" s="101" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="98" t="s">
+      <c r="A28" s="100" t="s">
         <v>184</v>
       </c>
-      <c r="B28" s="98" t="s">
+      <c r="B28" s="100" t="s">
         <v>147</v>
       </c>
-      <c r="C28" s="98" t="s">
+      <c r="C28" s="100" t="s">
         <v>207</v>
       </c>
-      <c r="D28" s="98" t="s">
+      <c r="D28" s="100" t="s">
         <v>47</v>
       </c>
-      <c r="E28" s="99" t="s">
-        <v>141</v>
-      </c>
-      <c r="F28" s="99" t="s">
+      <c r="E28" s="101" t="s">
+        <v>141</v>
+      </c>
+      <c r="F28" s="101" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="98" t="s">
+      <c r="A29" s="100" t="s">
         <v>184</v>
       </c>
-      <c r="B29" s="98" t="s">
+      <c r="B29" s="100" t="s">
         <v>147</v>
       </c>
-      <c r="C29" s="98" t="s">
+      <c r="C29" s="100" t="s">
         <v>203</v>
       </c>
-      <c r="D29" s="98" t="s">
+      <c r="D29" s="100" t="s">
         <v>46</v>
       </c>
-      <c r="E29" s="99" t="s">
-        <v>141</v>
-      </c>
-      <c r="F29" s="99" t="s">
+      <c r="E29" s="101" t="s">
+        <v>141</v>
+      </c>
+      <c r="F29" s="101" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="98" t="s">
+      <c r="A30" s="100" t="s">
         <v>184</v>
       </c>
-      <c r="B30" s="98" t="s">
+      <c r="B30" s="100" t="s">
         <v>147</v>
       </c>
-      <c r="C30" s="98" t="s">
+      <c r="C30" s="100" t="s">
         <v>204</v>
       </c>
-      <c r="D30" s="98" t="s">
+      <c r="D30" s="100" t="s">
         <v>43</v>
       </c>
-      <c r="E30" s="99" t="s">
-        <v>141</v>
-      </c>
-      <c r="F30" s="99" t="s">
+      <c r="E30" s="101" t="s">
+        <v>141</v>
+      </c>
+      <c r="F30" s="101" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="98" t="s">
+      <c r="A31" s="100" t="s">
         <v>185</v>
       </c>
-      <c r="B31" s="98" t="s">
+      <c r="B31" s="100" t="s">
         <v>70</v>
       </c>
-      <c r="C31" s="98" t="s">
+      <c r="C31" s="100" t="s">
         <v>215</v>
       </c>
-      <c r="D31" s="98" t="s">
+      <c r="D31" s="100" t="s">
         <v>312</v>
       </c>
-      <c r="E31" s="99" t="s">
-        <v>141</v>
-      </c>
-      <c r="F31" s="99" t="s">
+      <c r="E31" s="101" t="s">
+        <v>141</v>
+      </c>
+      <c r="F31" s="101" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="98" t="s">
+      <c r="A32" s="100" t="s">
         <v>185</v>
       </c>
-      <c r="B32" s="98" t="s">
+      <c r="B32" s="100" t="s">
         <v>70</v>
       </c>
-      <c r="C32" s="98" t="s">
+      <c r="C32" s="100" t="s">
         <v>216</v>
       </c>
-      <c r="D32" s="98" t="s">
+      <c r="D32" s="100" t="s">
         <v>157</v>
       </c>
-      <c r="E32" s="99" t="s">
-        <v>141</v>
-      </c>
-      <c r="F32" s="99" t="s">
+      <c r="E32" s="101" t="s">
+        <v>141</v>
+      </c>
+      <c r="F32" s="101" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="98" t="s">
+      <c r="A33" s="100" t="s">
         <v>185</v>
       </c>
-      <c r="B33" s="98" t="s">
+      <c r="B33" s="100" t="s">
         <v>70</v>
       </c>
-      <c r="C33" s="98" t="s">
+      <c r="C33" s="100" t="s">
         <v>214</v>
       </c>
-      <c r="D33" s="98" t="s">
+      <c r="D33" s="100" t="s">
         <v>76</v>
       </c>
-      <c r="E33" s="99" t="s">
-        <v>141</v>
-      </c>
-      <c r="F33" s="99" t="s">
+      <c r="E33" s="101" t="s">
+        <v>141</v>
+      </c>
+      <c r="F33" s="101" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="98" t="s">
+      <c r="A34" s="100" t="s">
         <v>185</v>
       </c>
-      <c r="B34" s="98" t="s">
+      <c r="B34" s="100" t="s">
         <v>70</v>
       </c>
-      <c r="C34" s="98" t="s">
+      <c r="C34" s="100" t="s">
         <v>213</v>
       </c>
-      <c r="D34" s="98" t="s">
+      <c r="D34" s="100" t="s">
         <v>75</v>
       </c>
-      <c r="E34" s="99" t="s">
-        <v>141</v>
-      </c>
-      <c r="F34" s="99" t="s">
+      <c r="E34" s="101" t="s">
+        <v>141</v>
+      </c>
+      <c r="F34" s="101" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="98" t="s">
+      <c r="A35" s="100" t="s">
         <v>185</v>
       </c>
-      <c r="B35" s="98" t="s">
+      <c r="B35" s="100" t="s">
         <v>70</v>
       </c>
-      <c r="C35" s="98" t="s">
+      <c r="C35" s="100" t="s">
         <v>209</v>
       </c>
-      <c r="D35" s="98" t="s">
+      <c r="D35" s="100" t="s">
         <v>74</v>
       </c>
-      <c r="E35" s="99" t="s">
-        <v>141</v>
-      </c>
-      <c r="F35" s="99" t="s">
+      <c r="E35" s="101" t="s">
+        <v>141</v>
+      </c>
+      <c r="F35" s="101" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="98" t="s">
+      <c r="A36" s="100" t="s">
         <v>185</v>
       </c>
-      <c r="B36" s="98" t="s">
+      <c r="B36" s="100" t="s">
         <v>70</v>
       </c>
-      <c r="C36" s="98" t="s">
+      <c r="C36" s="100" t="s">
         <v>212</v>
       </c>
-      <c r="D36" s="98" t="s">
+      <c r="D36" s="100" t="s">
         <v>156</v>
       </c>
-      <c r="E36" s="99" t="s">
-        <v>141</v>
-      </c>
-      <c r="F36" s="99" t="s">
+      <c r="E36" s="101" t="s">
+        <v>141</v>
+      </c>
+      <c r="F36" s="101" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="98" t="s">
+      <c r="A37" s="100" t="s">
         <v>185</v>
       </c>
-      <c r="B37" s="98" t="s">
+      <c r="B37" s="100" t="s">
         <v>70</v>
       </c>
-      <c r="C37" s="98" t="s">
+      <c r="C37" s="100" t="s">
         <v>211</v>
       </c>
-      <c r="D37" s="98" t="s">
+      <c r="D37" s="100" t="s">
         <v>72</v>
       </c>
-      <c r="E37" s="99" t="s">
-        <v>141</v>
-      </c>
-      <c r="F37" s="99" t="s">
+      <c r="E37" s="101" t="s">
+        <v>141</v>
+      </c>
+      <c r="F37" s="101" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="98" t="s">
+      <c r="A38" s="100" t="s">
         <v>185</v>
       </c>
-      <c r="B38" s="98" t="s">
+      <c r="B38" s="100" t="s">
         <v>70</v>
       </c>
-      <c r="C38" s="98" t="s">
+      <c r="C38" s="100" t="s">
         <v>210</v>
       </c>
-      <c r="D38" s="98" t="s">
+      <c r="D38" s="100" t="s">
         <v>71</v>
       </c>
-      <c r="E38" s="99" t="s">
-        <v>141</v>
-      </c>
-      <c r="F38" s="99" t="s">
+      <c r="E38" s="101" t="s">
+        <v>141</v>
+      </c>
+      <c r="F38" s="101" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="98" t="s">
+      <c r="A39" s="100" t="s">
         <v>181</v>
       </c>
-      <c r="B39" s="98" t="s">
+      <c r="B39" s="100" t="s">
         <v>77</v>
       </c>
-      <c r="C39" s="98" t="s">
+      <c r="C39" s="100" t="s">
         <v>221</v>
       </c>
-      <c r="D39" s="98" t="s">
+      <c r="D39" s="100" t="s">
         <v>79</v>
       </c>
-      <c r="E39" s="99" t="s">
-        <v>141</v>
-      </c>
-      <c r="F39" s="99" t="s">
+      <c r="E39" s="101" t="s">
+        <v>141</v>
+      </c>
+      <c r="F39" s="101" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="98" t="s">
+      <c r="A40" s="100" t="s">
         <v>181</v>
       </c>
-      <c r="B40" s="98" t="s">
+      <c r="B40" s="100" t="s">
         <v>77</v>
       </c>
-      <c r="C40" s="98" t="s">
+      <c r="C40" s="100" t="s">
         <v>222</v>
       </c>
-      <c r="D40" s="98" t="s">
+      <c r="D40" s="100" t="s">
         <v>82</v>
       </c>
-      <c r="E40" s="99" t="s">
-        <v>141</v>
-      </c>
-      <c r="F40" s="99" t="s">
+      <c r="E40" s="101" t="s">
+        <v>141</v>
+      </c>
+      <c r="F40" s="101" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="98" t="s">
+      <c r="A41" s="100" t="s">
         <v>181</v>
       </c>
-      <c r="B41" s="98" t="s">
+      <c r="B41" s="100" t="s">
         <v>77</v>
       </c>
-      <c r="C41" s="98" t="s">
+      <c r="C41" s="100" t="s">
         <v>220</v>
       </c>
-      <c r="D41" s="98" t="s">
+      <c r="D41" s="100" t="s">
         <v>158</v>
       </c>
-      <c r="E41" s="99" t="s">
-        <v>141</v>
-      </c>
-      <c r="F41" s="99" t="s">
+      <c r="E41" s="101" t="s">
+        <v>141</v>
+      </c>
+      <c r="F41" s="101" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="98" t="s">
+      <c r="A42" s="100" t="s">
         <v>181</v>
       </c>
-      <c r="B42" s="98" t="s">
+      <c r="B42" s="100" t="s">
         <v>77</v>
       </c>
-      <c r="C42" s="98" t="s">
+      <c r="C42" s="100" t="s">
         <v>217</v>
       </c>
-      <c r="D42" s="98" t="s">
+      <c r="D42" s="100" t="s">
         <v>78</v>
       </c>
-      <c r="E42" s="99" t="s">
-        <v>141</v>
-      </c>
-      <c r="F42" s="99" t="s">
+      <c r="E42" s="101" t="s">
+        <v>141</v>
+      </c>
+      <c r="F42" s="101" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="98" t="s">
+      <c r="A43" s="100" t="s">
         <v>181</v>
       </c>
-      <c r="B43" s="98" t="s">
+      <c r="B43" s="100" t="s">
         <v>77</v>
       </c>
-      <c r="C43" s="98" t="s">
+      <c r="C43" s="100" t="s">
         <v>219</v>
       </c>
-      <c r="D43" s="98" t="s">
+      <c r="D43" s="100" t="s">
         <v>313</v>
       </c>
-      <c r="E43" s="99" t="s">
-        <v>141</v>
-      </c>
-      <c r="F43" s="99" t="s">
+      <c r="E43" s="101" t="s">
+        <v>141</v>
+      </c>
+      <c r="F43" s="101" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="98" t="s">
+      <c r="A44" s="100" t="s">
         <v>181</v>
       </c>
-      <c r="B44" s="98" t="s">
+      <c r="B44" s="100" t="s">
         <v>77</v>
       </c>
-      <c r="C44" s="98" t="s">
+      <c r="C44" s="100" t="s">
         <v>218</v>
       </c>
-      <c r="D44" s="98" t="s">
+      <c r="D44" s="100" t="s">
         <v>314</v>
       </c>
-      <c r="E44" s="99" t="s">
-        <v>141</v>
-      </c>
-      <c r="F44" s="99" t="s">
+      <c r="E44" s="101" t="s">
+        <v>141</v>
+      </c>
+      <c r="F44" s="101" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="98" t="s">
+      <c r="A45" s="100" t="s">
         <v>186</v>
       </c>
-      <c r="B45" s="98" t="s">
+      <c r="B45" s="100" t="s">
         <v>159</v>
       </c>
-      <c r="C45" s="98" t="s">
+      <c r="C45" s="100" t="s">
         <v>224</v>
       </c>
-      <c r="D45" s="98" t="s">
+      <c r="D45" s="100" t="s">
         <v>84</v>
       </c>
-      <c r="E45" s="99" t="s">
-        <v>141</v>
-      </c>
-      <c r="F45" s="99" t="s">
+      <c r="E45" s="101" t="s">
+        <v>141</v>
+      </c>
+      <c r="F45" s="101" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="98" t="s">
+      <c r="A46" s="100" t="s">
         <v>186</v>
       </c>
-      <c r="B46" s="98" t="s">
+      <c r="B46" s="100" t="s">
         <v>159</v>
       </c>
-      <c r="C46" s="98" t="s">
+      <c r="C46" s="100" t="s">
         <v>225</v>
       </c>
-      <c r="D46" s="98" t="s">
+      <c r="D46" s="100" t="s">
         <v>96</v>
       </c>
-      <c r="E46" s="99" t="s">
-        <v>141</v>
-      </c>
-      <c r="F46" s="99" t="s">
+      <c r="E46" s="101" t="s">
+        <v>141</v>
+      </c>
+      <c r="F46" s="101" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" s="98" t="s">
+      <c r="A47" s="100" t="s">
         <v>186</v>
       </c>
-      <c r="B47" s="98" t="s">
+      <c r="B47" s="100" t="s">
         <v>159</v>
       </c>
-      <c r="C47" s="98" t="s">
+      <c r="C47" s="100" t="s">
         <v>231</v>
       </c>
-      <c r="D47" s="98" t="s">
+      <c r="D47" s="100" t="s">
         <v>168</v>
       </c>
-      <c r="E47" s="99" t="s">
-        <v>141</v>
-      </c>
-      <c r="F47" s="99" t="s">
+      <c r="E47" s="101" t="s">
+        <v>141</v>
+      </c>
+      <c r="F47" s="101" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="98" t="s">
+      <c r="A48" s="100" t="s">
         <v>186</v>
       </c>
-      <c r="B48" s="98" t="s">
+      <c r="B48" s="100" t="s">
         <v>159</v>
       </c>
-      <c r="C48" s="98" t="s">
+      <c r="C48" s="100" t="s">
         <v>232</v>
       </c>
-      <c r="D48" s="98" t="s">
+      <c r="D48" s="100" t="s">
         <v>167</v>
       </c>
-      <c r="E48" s="99" t="s">
-        <v>141</v>
-      </c>
-      <c r="F48" s="99" t="s">
+      <c r="E48" s="101" t="s">
+        <v>141</v>
+      </c>
+      <c r="F48" s="101" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="98" t="s">
+      <c r="A49" s="100" t="s">
         <v>186</v>
       </c>
-      <c r="B49" s="98" t="s">
+      <c r="B49" s="100" t="s">
         <v>159</v>
       </c>
-      <c r="C49" s="98" t="s">
+      <c r="C49" s="100" t="s">
         <v>233</v>
       </c>
-      <c r="D49" s="98" t="s">
+      <c r="D49" s="100" t="s">
         <v>166</v>
       </c>
-      <c r="E49" s="99" t="s">
-        <v>141</v>
-      </c>
-      <c r="F49" s="99" t="s">
+      <c r="E49" s="101" t="s">
+        <v>141</v>
+      </c>
+      <c r="F49" s="101" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="98" t="s">
+      <c r="A50" s="100" t="s">
         <v>186</v>
       </c>
-      <c r="B50" s="98" t="s">
+      <c r="B50" s="100" t="s">
         <v>159</v>
       </c>
-      <c r="C50" s="98" t="s">
+      <c r="C50" s="100" t="s">
         <v>234</v>
       </c>
-      <c r="D50" s="98" t="s">
+      <c r="D50" s="100" t="s">
         <v>165</v>
       </c>
-      <c r="E50" s="99" t="s">
-        <v>141</v>
-      </c>
-      <c r="F50" s="99" t="s">
+      <c r="E50" s="101" t="s">
+        <v>141</v>
+      </c>
+      <c r="F50" s="101" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" s="98" t="s">
+      <c r="A51" s="100" t="s">
         <v>186</v>
       </c>
-      <c r="B51" s="98" t="s">
+      <c r="B51" s="100" t="s">
         <v>159</v>
       </c>
-      <c r="C51" s="98" t="s">
+      <c r="C51" s="100" t="s">
         <v>235</v>
       </c>
-      <c r="D51" s="98" t="s">
+      <c r="D51" s="100" t="s">
         <v>164</v>
       </c>
-      <c r="E51" s="99" t="s">
-        <v>141</v>
-      </c>
-      <c r="F51" s="99" t="s">
+      <c r="E51" s="101" t="s">
+        <v>141</v>
+      </c>
+      <c r="F51" s="101" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" s="98" t="s">
+      <c r="A52" s="100" t="s">
         <v>186</v>
       </c>
-      <c r="B52" s="98" t="s">
+      <c r="B52" s="100" t="s">
         <v>159</v>
       </c>
-      <c r="C52" s="98" t="s">
+      <c r="C52" s="100" t="s">
         <v>228</v>
       </c>
-      <c r="D52" s="98" t="s">
+      <c r="D52" s="100" t="s">
         <v>163</v>
       </c>
-      <c r="E52" s="99" t="s">
-        <v>141</v>
-      </c>
-      <c r="F52" s="99" t="s">
+      <c r="E52" s="101" t="s">
+        <v>141</v>
+      </c>
+      <c r="F52" s="101" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" s="98" t="s">
+      <c r="A53" s="100" t="s">
         <v>186</v>
       </c>
-      <c r="B53" s="98" t="s">
+      <c r="B53" s="100" t="s">
         <v>159</v>
       </c>
-      <c r="C53" s="98" t="s">
+      <c r="C53" s="100" t="s">
         <v>229</v>
       </c>
-      <c r="D53" s="98" t="s">
+      <c r="D53" s="100" t="s">
         <v>162</v>
       </c>
-      <c r="E53" s="99" t="s">
-        <v>141</v>
-      </c>
-      <c r="F53" s="99" t="s">
+      <c r="E53" s="101" t="s">
+        <v>141</v>
+      </c>
+      <c r="F53" s="101" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" s="98" t="s">
+      <c r="A54" s="100" t="s">
         <v>186</v>
       </c>
-      <c r="B54" s="98" t="s">
+      <c r="B54" s="100" t="s">
         <v>159</v>
       </c>
-      <c r="C54" s="98" t="s">
+      <c r="C54" s="100" t="s">
         <v>230</v>
       </c>
-      <c r="D54" s="98" t="s">
+      <c r="D54" s="100" t="s">
         <v>88</v>
       </c>
-      <c r="E54" s="99" t="s">
-        <v>141</v>
-      </c>
-      <c r="F54" s="99" t="s">
+      <c r="E54" s="101" t="s">
+        <v>141</v>
+      </c>
+      <c r="F54" s="101" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" s="98" t="s">
+      <c r="A55" s="100" t="s">
         <v>186</v>
       </c>
-      <c r="B55" s="98" t="s">
+      <c r="B55" s="100" t="s">
         <v>159</v>
       </c>
-      <c r="C55" s="98" t="s">
+      <c r="C55" s="100" t="s">
         <v>223</v>
       </c>
-      <c r="D55" s="98" t="s">
+      <c r="D55" s="100" t="s">
         <v>161</v>
       </c>
-      <c r="E55" s="99" t="s">
-        <v>141</v>
-      </c>
-      <c r="F55" s="99" t="s">
+      <c r="E55" s="101" t="s">
+        <v>141</v>
+      </c>
+      <c r="F55" s="101" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" s="98" t="s">
+      <c r="A56" s="100" t="s">
         <v>186</v>
       </c>
-      <c r="B56" s="98" t="s">
+      <c r="B56" s="100" t="s">
         <v>159</v>
       </c>
-      <c r="C56" s="98" t="s">
+      <c r="C56" s="100" t="s">
         <v>227</v>
       </c>
-      <c r="D56" s="98" t="s">
+      <c r="D56" s="100" t="s">
         <v>86</v>
       </c>
-      <c r="E56" s="99" t="s">
-        <v>141</v>
-      </c>
-      <c r="F56" s="99" t="s">
+      <c r="E56" s="101" t="s">
+        <v>141</v>
+      </c>
+      <c r="F56" s="101" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57" s="98" t="s">
+      <c r="A57" s="100" t="s">
         <v>186</v>
       </c>
-      <c r="B57" s="98" t="s">
+      <c r="B57" s="100" t="s">
         <v>159</v>
       </c>
-      <c r="C57" s="98" t="s">
+      <c r="C57" s="100" t="s">
         <v>226</v>
       </c>
-      <c r="D57" s="98" t="s">
+      <c r="D57" s="100" t="s">
         <v>160</v>
       </c>
-      <c r="E57" s="99" t="s">
-        <v>141</v>
-      </c>
-      <c r="F57" s="99" t="s">
+      <c r="E57" s="101" t="s">
+        <v>141</v>
+      </c>
+      <c r="F57" s="101" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" s="98" t="s">
+      <c r="A58" s="100" t="s">
         <v>189</v>
       </c>
-      <c r="B58" s="98" t="s">
+      <c r="B58" s="100" t="s">
         <v>169</v>
       </c>
-      <c r="C58" s="98" t="s">
+      <c r="C58" s="100" t="s">
         <v>238</v>
       </c>
-      <c r="D58" s="98" t="s">
+      <c r="D58" s="100" t="s">
         <v>315</v>
       </c>
-      <c r="E58" s="99" t="s">
-        <v>141</v>
-      </c>
-      <c r="F58" s="99" t="s">
+      <c r="E58" s="101" t="s">
+        <v>141</v>
+      </c>
+      <c r="F58" s="101" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59" s="98" t="s">
+      <c r="A59" s="100" t="s">
         <v>189</v>
       </c>
-      <c r="B59" s="98" t="s">
+      <c r="B59" s="100" t="s">
         <v>169</v>
       </c>
-      <c r="C59" s="98" t="s">
+      <c r="C59" s="100" t="s">
         <v>237</v>
       </c>
-      <c r="D59" s="98" t="s">
+      <c r="D59" s="100" t="s">
         <v>316</v>
       </c>
-      <c r="E59" s="99" t="s">
-        <v>141</v>
-      </c>
-      <c r="F59" s="99" t="s">
+      <c r="E59" s="101" t="s">
+        <v>141</v>
+      </c>
+      <c r="F59" s="101" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A60" s="98" t="s">
+      <c r="A60" s="100" t="s">
         <v>189</v>
       </c>
-      <c r="B60" s="98" t="s">
+      <c r="B60" s="100" t="s">
         <v>169</v>
       </c>
-      <c r="C60" s="98" t="s">
+      <c r="C60" s="100" t="s">
         <v>241</v>
       </c>
-      <c r="D60" s="98" t="s">
+      <c r="D60" s="100" t="s">
         <v>99</v>
       </c>
-      <c r="E60" s="99" t="s">
-        <v>141</v>
-      </c>
-      <c r="F60" s="99" t="s">
+      <c r="E60" s="101" t="s">
+        <v>141</v>
+      </c>
+      <c r="F60" s="101" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A61" s="98" t="s">
+      <c r="A61" s="100" t="s">
         <v>189</v>
       </c>
-      <c r="B61" s="98" t="s">
+      <c r="B61" s="100" t="s">
         <v>169</v>
       </c>
-      <c r="C61" s="98" t="s">
+      <c r="C61" s="100" t="s">
         <v>236</v>
       </c>
-      <c r="D61" s="98" t="s">
+      <c r="D61" s="100" t="s">
         <v>98</v>
       </c>
-      <c r="E61" s="99" t="s">
-        <v>141</v>
-      </c>
-      <c r="F61" s="99" t="s">
+      <c r="E61" s="101" t="s">
+        <v>141</v>
+      </c>
+      <c r="F61" s="101" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A62" s="98" t="s">
+      <c r="A62" s="100" t="s">
         <v>189</v>
       </c>
-      <c r="B62" s="98" t="s">
+      <c r="B62" s="100" t="s">
         <v>169</v>
       </c>
-      <c r="C62" s="98" t="s">
+      <c r="C62" s="100" t="s">
         <v>240</v>
       </c>
-      <c r="D62" s="98" t="s">
+      <c r="D62" s="100" t="s">
         <v>171</v>
       </c>
-      <c r="E62" s="99" t="s">
-        <v>141</v>
-      </c>
-      <c r="F62" s="99" t="s">
+      <c r="E62" s="101" t="s">
+        <v>141</v>
+      </c>
+      <c r="F62" s="101" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A63" s="98" t="s">
+      <c r="A63" s="100" t="s">
         <v>189</v>
       </c>
-      <c r="B63" s="98" t="s">
+      <c r="B63" s="100" t="s">
         <v>169</v>
       </c>
-      <c r="C63" s="98" t="s">
+      <c r="C63" s="100" t="s">
         <v>242</v>
       </c>
-      <c r="D63" s="98" t="s">
+      <c r="D63" s="100" t="s">
         <v>170</v>
       </c>
-      <c r="E63" s="99" t="s">
-        <v>141</v>
-      </c>
-      <c r="F63" s="99" t="s">
+      <c r="E63" s="101" t="s">
+        <v>141</v>
+      </c>
+      <c r="F63" s="101" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A64" s="98" t="s">
+      <c r="A64" s="100" t="s">
         <v>189</v>
       </c>
-      <c r="B64" s="98" t="s">
+      <c r="B64" s="100" t="s">
         <v>169</v>
       </c>
-      <c r="C64" s="98" t="s">
+      <c r="C64" s="100" t="s">
         <v>239</v>
       </c>
-      <c r="D64" s="98" t="s">
+      <c r="D64" s="100" t="s">
         <v>317</v>
       </c>
-      <c r="E64" s="99" t="s">
-        <v>141</v>
-      </c>
-      <c r="F64" s="99" t="s">
+      <c r="E64" s="101" t="s">
+        <v>141</v>
+      </c>
+      <c r="F64" s="101" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A65" s="98" t="s">
+      <c r="A65" s="100" t="s">
         <v>198</v>
       </c>
-      <c r="B65" s="98" t="s">
+      <c r="B65" s="100" t="s">
         <v>172</v>
       </c>
-      <c r="C65" s="98" t="s">
+      <c r="C65" s="100" t="s">
         <v>250</v>
       </c>
-      <c r="D65" s="98" t="s">
+      <c r="D65" s="100" t="s">
         <v>318</v>
       </c>
-      <c r="E65" s="99" t="s">
-        <v>141</v>
-      </c>
-      <c r="F65" s="99" t="s">
+      <c r="E65" s="101" t="s">
+        <v>141</v>
+      </c>
+      <c r="F65" s="101" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A66" s="98" t="s">
+      <c r="A66" s="100" t="s">
         <v>198</v>
       </c>
-      <c r="B66" s="98" t="s">
+      <c r="B66" s="100" t="s">
         <v>172</v>
       </c>
-      <c r="C66" s="98" t="s">
+      <c r="C66" s="100" t="s">
         <v>247</v>
       </c>
-      <c r="D66" s="98" t="s">
+      <c r="D66" s="100" t="s">
         <v>175</v>
       </c>
-      <c r="E66" s="99" t="s">
-        <v>141</v>
-      </c>
-      <c r="F66" s="99" t="s">
+      <c r="E66" s="101" t="s">
+        <v>141</v>
+      </c>
+      <c r="F66" s="101" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A67" s="98" t="s">
+      <c r="A67" s="100" t="s">
         <v>198</v>
       </c>
-      <c r="B67" s="98" t="s">
+      <c r="B67" s="100" t="s">
         <v>172</v>
       </c>
-      <c r="C67" s="98" t="s">
+      <c r="C67" s="100" t="s">
         <v>246</v>
       </c>
-      <c r="D67" s="98" t="s">
+      <c r="D67" s="100" t="s">
         <v>106</v>
       </c>
-      <c r="E67" s="99" t="s">
-        <v>141</v>
-      </c>
-      <c r="F67" s="99" t="s">
+      <c r="E67" s="101" t="s">
+        <v>141</v>
+      </c>
+      <c r="F67" s="101" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A68" s="98" t="s">
+      <c r="A68" s="100" t="s">
         <v>198</v>
       </c>
-      <c r="B68" s="98" t="s">
+      <c r="B68" s="100" t="s">
         <v>172</v>
       </c>
-      <c r="C68" s="98" t="s">
+      <c r="C68" s="100" t="s">
         <v>245</v>
       </c>
-      <c r="D68" s="98" t="s">
+      <c r="D68" s="100" t="s">
         <v>174</v>
       </c>
-      <c r="E68" s="99" t="s">
-        <v>141</v>
-      </c>
-      <c r="F68" s="99" t="s">
+      <c r="E68" s="101" t="s">
+        <v>141</v>
+      </c>
+      <c r="F68" s="101" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A69" s="98" t="s">
+      <c r="A69" s="100" t="s">
         <v>198</v>
       </c>
-      <c r="B69" s="98" t="s">
+      <c r="B69" s="100" t="s">
         <v>172</v>
       </c>
-      <c r="C69" s="98" t="s">
+      <c r="C69" s="100" t="s">
         <v>244</v>
       </c>
-      <c r="D69" s="98" t="s">
+      <c r="D69" s="100" t="s">
         <v>173</v>
       </c>
-      <c r="E69" s="99" t="s">
-        <v>141</v>
-      </c>
-      <c r="F69" s="99" t="s">
+      <c r="E69" s="101" t="s">
+        <v>141</v>
+      </c>
+      <c r="F69" s="101" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A70" s="98" t="s">
+      <c r="A70" s="100" t="s">
         <v>198</v>
       </c>
-      <c r="B70" s="98" t="s">
+      <c r="B70" s="100" t="s">
         <v>172</v>
       </c>
-      <c r="C70" s="98" t="s">
+      <c r="C70" s="100" t="s">
         <v>243</v>
       </c>
-      <c r="D70" s="98" t="s">
+      <c r="D70" s="100" t="s">
         <v>319</v>
       </c>
-      <c r="E70" s="99" t="s">
-        <v>141</v>
-      </c>
-      <c r="F70" s="99" t="s">
+      <c r="E70" s="101" t="s">
+        <v>141</v>
+      </c>
+      <c r="F70" s="101" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A71" s="98" t="s">
+      <c r="A71" s="100" t="s">
         <v>198</v>
       </c>
-      <c r="B71" s="98" t="s">
+      <c r="B71" s="100" t="s">
         <v>172</v>
       </c>
-      <c r="C71" s="98" t="s">
+      <c r="C71" s="100" t="s">
         <v>249</v>
       </c>
-      <c r="D71" s="98" t="s">
+      <c r="D71" s="100" t="s">
         <v>177</v>
       </c>
-      <c r="E71" s="99" t="s">
-        <v>141</v>
-      </c>
-      <c r="F71" s="99" t="s">
+      <c r="E71" s="101" t="s">
+        <v>141</v>
+      </c>
+      <c r="F71" s="101" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A72" s="98" t="s">
+      <c r="A72" s="100" t="s">
         <v>198</v>
       </c>
-      <c r="B72" s="98" t="s">
+      <c r="B72" s="100" t="s">
         <v>172</v>
       </c>
-      <c r="C72" s="98" t="s">
+      <c r="C72" s="100" t="s">
         <v>251</v>
       </c>
-      <c r="D72" s="98" t="s">
+      <c r="D72" s="100" t="s">
         <v>320</v>
       </c>
-      <c r="E72" s="99" t="s">
-        <v>141</v>
-      </c>
-      <c r="F72" s="99" t="s">
+      <c r="E72" s="101" t="s">
+        <v>141</v>
+      </c>
+      <c r="F72" s="101" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A73" s="98" t="s">
+      <c r="A73" s="100" t="s">
         <v>198</v>
       </c>
-      <c r="B73" s="98" t="s">
+      <c r="B73" s="100" t="s">
         <v>172</v>
       </c>
-      <c r="C73" s="98" t="s">
+      <c r="C73" s="100" t="s">
         <v>248</v>
       </c>
-      <c r="D73" s="98" t="s">
+      <c r="D73" s="100" t="s">
         <v>176</v>
       </c>
-      <c r="E73" s="99" t="s">
-        <v>141</v>
-      </c>
-      <c r="F73" s="99" t="s">
+      <c r="E73" s="101" t="s">
+        <v>141</v>
+      </c>
+      <c r="F73" s="101" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A74" s="98" t="s">
+      <c r="A74" s="100" t="s">
         <v>197</v>
       </c>
-      <c r="B74" s="98" t="s">
+      <c r="B74" s="100" t="s">
         <v>178</v>
       </c>
-      <c r="C74" s="98" t="s">
+      <c r="C74" s="100" t="s">
         <v>259</v>
       </c>
-      <c r="D74" s="98" t="s">
+      <c r="D74" s="100" t="s">
         <v>112</v>
       </c>
-      <c r="E74" s="99" t="s">
-        <v>141</v>
-      </c>
-      <c r="F74" s="99" t="s">
+      <c r="E74" s="101" t="s">
+        <v>141</v>
+      </c>
+      <c r="F74" s="101" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A75" s="98" t="s">
+      <c r="A75" s="100" t="s">
         <v>197</v>
       </c>
-      <c r="B75" s="98" t="s">
+      <c r="B75" s="100" t="s">
         <v>178</v>
       </c>
-      <c r="C75" s="98" t="s">
+      <c r="C75" s="100" t="s">
         <v>255</v>
       </c>
-      <c r="D75" s="98" t="s">
+      <c r="D75" s="100" t="s">
         <v>117</v>
       </c>
-      <c r="E75" s="99" t="s">
-        <v>141</v>
-      </c>
-      <c r="F75" s="99" t="s">
+      <c r="E75" s="101" t="s">
+        <v>141</v>
+      </c>
+      <c r="F75" s="101" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A76" s="98" t="s">
+      <c r="A76" s="100" t="s">
         <v>197</v>
       </c>
-      <c r="B76" s="98" t="s">
+      <c r="B76" s="100" t="s">
         <v>178</v>
       </c>
-      <c r="C76" s="98" t="s">
+      <c r="C76" s="100" t="s">
         <v>260</v>
       </c>
-      <c r="D76" s="98" t="s">
+      <c r="D76" s="100" t="s">
         <v>321</v>
       </c>
-      <c r="E76" s="99" t="s">
-        <v>141</v>
-      </c>
-      <c r="F76" s="99" t="s">
+      <c r="E76" s="101" t="s">
+        <v>141</v>
+      </c>
+      <c r="F76" s="101" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A77" s="98" t="s">
+      <c r="A77" s="100" t="s">
         <v>197</v>
       </c>
-      <c r="B77" s="98" t="s">
+      <c r="B77" s="100" t="s">
         <v>178</v>
       </c>
-      <c r="C77" s="98" t="s">
+      <c r="C77" s="100" t="s">
         <v>252</v>
       </c>
-      <c r="D77" s="98" t="s">
+      <c r="D77" s="100" t="s">
         <v>322</v>
       </c>
-      <c r="E77" s="99" t="s">
-        <v>141</v>
-      </c>
-      <c r="F77" s="99" t="s">
+      <c r="E77" s="101" t="s">
+        <v>141</v>
+      </c>
+      <c r="F77" s="101" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A78" s="98" t="s">
+      <c r="A78" s="100" t="s">
         <v>197</v>
       </c>
-      <c r="B78" s="98" t="s">
+      <c r="B78" s="100" t="s">
         <v>178</v>
       </c>
-      <c r="C78" s="98" t="s">
+      <c r="C78" s="100" t="s">
         <v>262</v>
       </c>
-      <c r="D78" s="98" t="s">
+      <c r="D78" s="100" t="s">
         <v>179</v>
       </c>
-      <c r="E78" s="99" t="s">
-        <v>141</v>
-      </c>
-      <c r="F78" s="99" t="s">
+      <c r="E78" s="101" t="s">
+        <v>141</v>
+      </c>
+      <c r="F78" s="101" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A79" s="98" t="s">
+      <c r="A79" s="100" t="s">
         <v>197</v>
       </c>
-      <c r="B79" s="98" t="s">
+      <c r="B79" s="100" t="s">
         <v>178</v>
       </c>
-      <c r="C79" s="98" t="s">
+      <c r="C79" s="100" t="s">
         <v>261</v>
       </c>
-      <c r="D79" s="98" t="s">
+      <c r="D79" s="100" t="s">
         <v>120</v>
       </c>
-      <c r="E79" s="99" t="s">
-        <v>141</v>
-      </c>
-      <c r="F79" s="99" t="s">
+      <c r="E79" s="101" t="s">
+        <v>141</v>
+      </c>
+      <c r="F79" s="101" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A80" s="98" t="s">
+      <c r="A80" s="100" t="s">
         <v>197</v>
       </c>
-      <c r="B80" s="98" t="s">
+      <c r="B80" s="100" t="s">
         <v>178</v>
       </c>
-      <c r="C80" s="98" t="s">
+      <c r="C80" s="100" t="s">
         <v>254</v>
       </c>
-      <c r="D80" s="98" t="s">
+      <c r="D80" s="100" t="s">
         <v>323</v>
       </c>
-      <c r="E80" s="99" t="s">
-        <v>141</v>
-      </c>
-      <c r="F80" s="99" t="s">
+      <c r="E80" s="101" t="s">
+        <v>141</v>
+      </c>
+      <c r="F80" s="101" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A81" s="98" t="s">
+      <c r="A81" s="100" t="s">
         <v>197</v>
       </c>
-      <c r="B81" s="98" t="s">
+      <c r="B81" s="100" t="s">
         <v>178</v>
       </c>
-      <c r="C81" s="98" t="s">
+      <c r="C81" s="100" t="s">
         <v>258</v>
       </c>
-      <c r="D81" s="98" t="s">
+      <c r="D81" s="100" t="s">
         <v>113</v>
       </c>
-      <c r="E81" s="99" t="s">
-        <v>141</v>
-      </c>
-      <c r="F81" s="99" t="s">
+      <c r="E81" s="101" t="s">
+        <v>141</v>
+      </c>
+      <c r="F81" s="101" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A82" s="98" t="s">
+      <c r="A82" s="100" t="s">
         <v>197</v>
       </c>
-      <c r="B82" s="98" t="s">
+      <c r="B82" s="100" t="s">
         <v>178</v>
       </c>
-      <c r="C82" s="98" t="s">
+      <c r="C82" s="100" t="s">
         <v>253</v>
       </c>
-      <c r="D82" s="98" t="s">
+      <c r="D82" s="100" t="s">
         <v>324</v>
       </c>
-      <c r="E82" s="99" t="s">
-        <v>141</v>
-      </c>
-      <c r="F82" s="99" t="s">
+      <c r="E82" s="101" t="s">
+        <v>141</v>
+      </c>
+      <c r="F82" s="101" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A83" s="98" t="s">
+      <c r="A83" s="100" t="s">
         <v>197</v>
       </c>
-      <c r="B83" s="98" t="s">
+      <c r="B83" s="100" t="s">
         <v>178</v>
       </c>
-      <c r="C83" s="98" t="s">
+      <c r="C83" s="100" t="s">
         <v>257</v>
       </c>
-      <c r="D83" s="98" t="s">
+      <c r="D83" s="100" t="s">
         <v>115</v>
       </c>
-      <c r="E83" s="99" t="s">
-        <v>141</v>
-      </c>
-      <c r="F83" s="99" t="s">
+      <c r="E83" s="101" t="s">
+        <v>141</v>
+      </c>
+      <c r="F83" s="101" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A84" s="98" t="s">
+      <c r="A84" s="100" t="s">
         <v>197</v>
       </c>
-      <c r="B84" s="98" t="s">
+      <c r="B84" s="100" t="s">
         <v>178</v>
       </c>
-      <c r="C84" s="98" t="s">
+      <c r="C84" s="100" t="s">
         <v>256</v>
       </c>
-      <c r="D84" s="98" t="s">
+      <c r="D84" s="100" t="s">
         <v>116</v>
       </c>
-      <c r="E84" s="99" t="s">
-        <v>141</v>
-      </c>
-      <c r="F84" s="99" t="s">
+      <c r="E84" s="101" t="s">
+        <v>141</v>
+      </c>
+      <c r="F84" s="101" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A85" s="98" t="s">
+      <c r="A85" s="100" t="s">
         <v>196</v>
       </c>
-      <c r="B85" s="98" t="s">
+      <c r="B85" s="100" t="s">
         <v>145</v>
       </c>
-      <c r="C85" s="98" t="s">
+      <c r="C85" s="100" t="s">
         <v>263</v>
       </c>
-      <c r="D85" s="98" t="s">
+      <c r="D85" s="100" t="s">
         <v>122</v>
       </c>
-      <c r="E85" s="99" t="s">
-        <v>141</v>
-      </c>
-      <c r="F85" s="99" t="s">
+      <c r="E85" s="101" t="s">
+        <v>141</v>
+      </c>
+      <c r="F85" s="101" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A86" s="98" t="s">
+      <c r="A86" s="100" t="s">
         <v>196</v>
       </c>
-      <c r="B86" s="98" t="s">
+      <c r="B86" s="100" t="s">
         <v>145</v>
       </c>
-      <c r="C86" s="98" t="s">
+      <c r="C86" s="100" t="s">
         <v>266</v>
       </c>
-      <c r="D86" s="98" t="s">
+      <c r="D86" s="100" t="s">
         <v>123</v>
       </c>
-      <c r="E86" s="99" t="s">
-        <v>141</v>
-      </c>
-      <c r="F86" s="99" t="s">
+      <c r="E86" s="101" t="s">
+        <v>141</v>
+      </c>
+      <c r="F86" s="101" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A87" s="98" t="s">
+      <c r="A87" s="100" t="s">
         <v>196</v>
       </c>
-      <c r="B87" s="98" t="s">
+      <c r="B87" s="100" t="s">
         <v>145</v>
       </c>
-      <c r="C87" s="98" t="s">
+      <c r="C87" s="100" t="s">
         <v>264</v>
       </c>
-      <c r="D87" s="98" t="s">
+      <c r="D87" s="100" t="s">
         <v>325</v>
       </c>
-      <c r="E87" s="99" t="s">
-        <v>141</v>
-      </c>
-      <c r="F87" s="99" t="s">
+      <c r="E87" s="101" t="s">
+        <v>141</v>
+      </c>
+      <c r="F87" s="101" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A88" s="98" t="s">
+      <c r="A88" s="100" t="s">
         <v>196</v>
       </c>
-      <c r="B88" s="98" t="s">
+      <c r="B88" s="100" t="s">
         <v>145</v>
       </c>
-      <c r="C88" s="98" t="s">
+      <c r="C88" s="100" t="s">
         <v>265</v>
       </c>
-      <c r="D88" s="98" t="s">
+      <c r="D88" s="100" t="s">
         <v>124</v>
       </c>
-      <c r="E88" s="99" t="s">
-        <v>141</v>
-      </c>
-      <c r="F88" s="99" t="s">
+      <c r="E88" s="101" t="s">
+        <v>141</v>
+      </c>
+      <c r="F88" s="101" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A89" s="98" t="s">
+      <c r="A89" s="100" t="s">
         <v>227</v>
       </c>
-      <c r="B89" s="98" t="s">
+      <c r="B89" s="100" t="s">
         <v>148</v>
       </c>
-      <c r="C89" s="98" t="s">
+      <c r="C89" s="100" t="s">
         <v>268</v>
       </c>
-      <c r="D89" s="98" t="s">
+      <c r="D89" s="100" t="s">
         <v>150</v>
       </c>
-      <c r="E89" s="99" t="s">
-        <v>141</v>
-      </c>
-      <c r="F89" s="99" t="s">
+      <c r="E89" s="101" t="s">
+        <v>141</v>
+      </c>
+      <c r="F89" s="101" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A90" s="98" t="s">
+      <c r="A90" s="100" t="s">
         <v>227</v>
       </c>
-      <c r="B90" s="98" t="s">
+      <c r="B90" s="100" t="s">
         <v>148</v>
       </c>
-      <c r="C90" s="98" t="s">
+      <c r="C90" s="100" t="s">
         <v>267</v>
       </c>
-      <c r="D90" s="98" t="s">
+      <c r="D90" s="100" t="s">
         <v>149</v>
       </c>
-      <c r="E90" s="99" t="s">
-        <v>141</v>
-      </c>
-      <c r="F90" s="99" t="s">
+      <c r="E90" s="101" t="s">
+        <v>141</v>
+      </c>
+      <c r="F90" s="101" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A91" s="98" t="s">
+      <c r="A91" s="100" t="s">
         <v>229</v>
       </c>
-      <c r="B91" s="98" t="s">
+      <c r="B91" s="100" t="s">
         <v>154</v>
       </c>
-      <c r="C91" s="98" t="s">
+      <c r="C91" s="100" t="s">
         <v>269</v>
       </c>
-      <c r="D91" s="98" t="s">
+      <c r="D91" s="100" t="s">
         <v>57</v>
       </c>
-      <c r="E91" s="99" t="s">
-        <v>141</v>
-      </c>
-      <c r="F91" s="99" t="s">
+      <c r="E91" s="101" t="s">
+        <v>141</v>
+      </c>
+      <c r="F91" s="101" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A92" s="98" t="s">
+      <c r="A92" s="100" t="s">
         <v>229</v>
       </c>
-      <c r="B92" s="98" t="s">
+      <c r="B92" s="100" t="s">
         <v>154</v>
       </c>
-      <c r="C92" s="98" t="s">
+      <c r="C92" s="100" t="s">
         <v>270</v>
       </c>
-      <c r="D92" s="98" t="s">
+      <c r="D92" s="100" t="s">
         <v>326</v>
       </c>
-      <c r="E92" s="99" t="s">
-        <v>141</v>
-      </c>
-      <c r="F92" s="99" t="s">
+      <c r="E92" s="101" t="s">
+        <v>141</v>
+      </c>
+      <c r="F92" s="101" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A93" s="98" t="s">
+      <c r="A93" s="100" t="s">
         <v>229</v>
       </c>
-      <c r="B93" s="98" t="s">
+      <c r="B93" s="100" t="s">
         <v>154</v>
       </c>
-      <c r="C93" s="98" t="s">
+      <c r="C93" s="100" t="s">
         <v>271</v>
       </c>
-      <c r="D93" s="98" t="s">
+      <c r="D93" s="100" t="s">
         <v>327</v>
       </c>
-      <c r="E93" s="99" t="s">
-        <v>141</v>
-      </c>
-      <c r="F93" s="99" t="s">
+      <c r="E93" s="101" t="s">
+        <v>141</v>
+      </c>
+      <c r="F93" s="101" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A94" s="98" t="s">
+      <c r="A94" s="100" t="s">
         <v>229</v>
       </c>
-      <c r="B94" s="98" t="s">
+      <c r="B94" s="100" t="s">
         <v>154</v>
       </c>
-      <c r="C94" s="98" t="s">
+      <c r="C94" s="100" t="s">
         <v>275</v>
       </c>
-      <c r="D94" s="98" t="s">
+      <c r="D94" s="100" t="s">
         <v>50</v>
       </c>
-      <c r="E94" s="99" t="s">
-        <v>141</v>
-      </c>
-      <c r="F94" s="99" t="s">
+      <c r="E94" s="101" t="s">
+        <v>141</v>
+      </c>
+      <c r="F94" s="101" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A95" s="98" t="s">
+      <c r="A95" s="100" t="s">
         <v>229</v>
       </c>
-      <c r="B95" s="98" t="s">
+      <c r="B95" s="100" t="s">
         <v>154</v>
       </c>
-      <c r="C95" s="98" t="s">
+      <c r="C95" s="100" t="s">
         <v>274</v>
       </c>
-      <c r="D95" s="98" t="s">
+      <c r="D95" s="100" t="s">
         <v>52</v>
       </c>
-      <c r="E95" s="99" t="s">
-        <v>141</v>
-      </c>
-      <c r="F95" s="99" t="s">
+      <c r="E95" s="101" t="s">
+        <v>141</v>
+      </c>
+      <c r="F95" s="101" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A96" s="98" t="s">
+      <c r="A96" s="100" t="s">
         <v>229</v>
       </c>
-      <c r="B96" s="98" t="s">
+      <c r="B96" s="100" t="s">
         <v>154</v>
       </c>
-      <c r="C96" s="98" t="s">
+      <c r="C96" s="100" t="s">
         <v>272</v>
       </c>
-      <c r="D96" s="98" t="s">
+      <c r="D96" s="100" t="s">
         <v>58</v>
       </c>
-      <c r="E96" s="99" t="s">
-        <v>141</v>
-      </c>
-      <c r="F96" s="99" t="s">
+      <c r="E96" s="101" t="s">
+        <v>141</v>
+      </c>
+      <c r="F96" s="101" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A97" s="98" t="s">
+      <c r="A97" s="100" t="s">
         <v>229</v>
       </c>
-      <c r="B97" s="98" t="s">
+      <c r="B97" s="100" t="s">
         <v>154</v>
       </c>
-      <c r="C97" s="98" t="s">
+      <c r="C97" s="100" t="s">
         <v>276</v>
       </c>
-      <c r="D97" s="98" t="s">
+      <c r="D97" s="100" t="s">
         <v>328</v>
       </c>
-      <c r="E97" s="99" t="s">
-        <v>141</v>
-      </c>
-      <c r="F97" s="99" t="s">
+      <c r="E97" s="101" t="s">
+        <v>141</v>
+      </c>
+      <c r="F97" s="101" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A98" s="98" t="s">
+      <c r="A98" s="100" t="s">
         <v>229</v>
       </c>
-      <c r="B98" s="98" t="s">
+      <c r="B98" s="100" t="s">
         <v>154</v>
       </c>
-      <c r="C98" s="98" t="s">
+      <c r="C98" s="100" t="s">
         <v>277</v>
       </c>
-      <c r="D98" s="98" t="s">
+      <c r="D98" s="100" t="s">
         <v>329</v>
       </c>
-      <c r="E98" s="99" t="s">
-        <v>141</v>
-      </c>
-      <c r="F98" s="99" t="s">
+      <c r="E98" s="101" t="s">
+        <v>141</v>
+      </c>
+      <c r="F98" s="101" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A99" s="98" t="s">
+      <c r="A99" s="100" t="s">
         <v>229</v>
       </c>
-      <c r="B99" s="98" t="s">
+      <c r="B99" s="100" t="s">
         <v>154</v>
       </c>
-      <c r="C99" s="98" t="s">
+      <c r="C99" s="100" t="s">
         <v>273</v>
       </c>
-      <c r="D99" s="98" t="s">
+      <c r="D99" s="100" t="s">
         <v>330</v>
       </c>
-      <c r="E99" s="99" t="s">
-        <v>141</v>
-      </c>
-      <c r="F99" s="99" t="s">
+      <c r="E99" s="101" t="s">
+        <v>141</v>
+      </c>
+      <c r="F99" s="101" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A100" s="98" t="s">
+      <c r="A100" s="100" t="s">
         <v>228</v>
       </c>
-      <c r="B100" s="98" t="s">
+      <c r="B100" s="100" t="s">
         <v>59</v>
       </c>
-      <c r="C100" s="98" t="s">
+      <c r="C100" s="100" t="s">
         <v>283</v>
       </c>
-      <c r="D100" s="98" t="s">
+      <c r="D100" s="100" t="s">
         <v>61</v>
       </c>
-      <c r="E100" s="99" t="s">
-        <v>141</v>
-      </c>
-      <c r="F100" s="99" t="s">
+      <c r="E100" s="101" t="s">
+        <v>141</v>
+      </c>
+      <c r="F100" s="101" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A101" s="98" t="s">
+      <c r="A101" s="100" t="s">
         <v>228</v>
       </c>
-      <c r="B101" s="98" t="s">
+      <c r="B101" s="100" t="s">
         <v>59</v>
       </c>
-      <c r="C101" s="98" t="s">
+      <c r="C101" s="100" t="s">
         <v>281</v>
       </c>
-      <c r="D101" s="98" t="s">
+      <c r="D101" s="100" t="s">
         <v>69</v>
       </c>
-      <c r="E101" s="99" t="s">
-        <v>141</v>
-      </c>
-      <c r="F101" s="99" t="s">
+      <c r="E101" s="101" t="s">
+        <v>141</v>
+      </c>
+      <c r="F101" s="101" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A102" s="98" t="s">
+      <c r="A102" s="100" t="s">
         <v>228</v>
       </c>
-      <c r="B102" s="98" t="s">
+      <c r="B102" s="100" t="s">
         <v>59</v>
       </c>
-      <c r="C102" s="98" t="s">
+      <c r="C102" s="100" t="s">
         <v>280</v>
       </c>
-      <c r="D102" s="98" t="s">
+      <c r="D102" s="100" t="s">
         <v>155</v>
       </c>
-      <c r="E102" s="99" t="s">
-        <v>141</v>
-      </c>
-      <c r="F102" s="99" t="s">
+      <c r="E102" s="101" t="s">
+        <v>141</v>
+      </c>
+      <c r="F102" s="101" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A103" s="98" t="s">
+      <c r="A103" s="100" t="s">
         <v>228</v>
       </c>
-      <c r="B103" s="98" t="s">
+      <c r="B103" s="100" t="s">
         <v>59</v>
       </c>
-      <c r="C103" s="98" t="s">
+      <c r="C103" s="100" t="s">
         <v>279</v>
       </c>
-      <c r="D103" s="98" t="s">
+      <c r="D103" s="100" t="s">
         <v>67</v>
       </c>
-      <c r="E103" s="99" t="s">
-        <v>141</v>
-      </c>
-      <c r="F103" s="99" t="s">
+      <c r="E103" s="101" t="s">
+        <v>141</v>
+      </c>
+      <c r="F103" s="101" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A104" s="98" t="s">
+      <c r="A104" s="100" t="s">
         <v>228</v>
       </c>
-      <c r="B104" s="98" t="s">
+      <c r="B104" s="100" t="s">
         <v>59</v>
       </c>
-      <c r="C104" s="98" t="s">
+      <c r="C104" s="100" t="s">
         <v>278</v>
       </c>
-      <c r="D104" s="98" t="s">
+      <c r="D104" s="100" t="s">
         <v>66</v>
       </c>
-      <c r="E104" s="99" t="s">
-        <v>141</v>
-      </c>
-      <c r="F104" s="99" t="s">
+      <c r="E104" s="101" t="s">
+        <v>141</v>
+      </c>
+      <c r="F104" s="101" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A105" s="98" t="s">
+      <c r="A105" s="100" t="s">
         <v>228</v>
       </c>
-      <c r="B105" s="98" t="s">
+      <c r="B105" s="100" t="s">
         <v>59</v>
       </c>
-      <c r="C105" s="98" t="s">
+      <c r="C105" s="100" t="s">
         <v>287</v>
       </c>
-      <c r="D105" s="98" t="s">
+      <c r="D105" s="100" t="s">
         <v>65</v>
       </c>
-      <c r="E105" s="99" t="s">
-        <v>141</v>
-      </c>
-      <c r="F105" s="99" t="s">
+      <c r="E105" s="101" t="s">
+        <v>141</v>
+      </c>
+      <c r="F105" s="101" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A106" s="98" t="s">
+      <c r="A106" s="100" t="s">
         <v>228</v>
       </c>
-      <c r="B106" s="98" t="s">
+      <c r="B106" s="100" t="s">
         <v>59</v>
       </c>
-      <c r="C106" s="98" t="s">
+      <c r="C106" s="100" t="s">
         <v>286</v>
       </c>
-      <c r="D106" s="98" t="s">
+      <c r="D106" s="100" t="s">
         <v>64</v>
       </c>
-      <c r="E106" s="99" t="s">
-        <v>141</v>
-      </c>
-      <c r="F106" s="99" t="s">
+      <c r="E106" s="101" t="s">
+        <v>141</v>
+      </c>
+      <c r="F106" s="101" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A107" s="98" t="s">
+      <c r="A107" s="100" t="s">
         <v>228</v>
       </c>
-      <c r="B107" s="98" t="s">
+      <c r="B107" s="100" t="s">
         <v>59</v>
       </c>
-      <c r="C107" s="98" t="s">
+      <c r="C107" s="100" t="s">
         <v>285</v>
       </c>
-      <c r="D107" s="98" t="s">
+      <c r="D107" s="100" t="s">
         <v>63</v>
       </c>
-      <c r="E107" s="99" t="s">
-        <v>141</v>
-      </c>
-      <c r="F107" s="99" t="s">
+      <c r="E107" s="101" t="s">
+        <v>141</v>
+      </c>
+      <c r="F107" s="101" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A108" s="98" t="s">
+      <c r="A108" s="100" t="s">
         <v>228</v>
       </c>
-      <c r="B108" s="98" t="s">
+      <c r="B108" s="100" t="s">
         <v>59</v>
       </c>
-      <c r="C108" s="98" t="s">
+      <c r="C108" s="100" t="s">
         <v>284</v>
       </c>
-      <c r="D108" s="98" t="s">
+      <c r="D108" s="100" t="s">
         <v>62</v>
       </c>
-      <c r="E108" s="99" t="s">
-        <v>141</v>
-      </c>
-      <c r="F108" s="99" t="s">
+      <c r="E108" s="101" t="s">
+        <v>141</v>
+      </c>
+      <c r="F108" s="101" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A109" s="98" t="s">
+      <c r="A109" s="100" t="s">
         <v>228</v>
       </c>
-      <c r="B109" s="98" t="s">
+      <c r="B109" s="100" t="s">
         <v>59</v>
       </c>
-      <c r="C109" s="98" t="s">
+      <c r="C109" s="100" t="s">
         <v>282</v>
       </c>
-      <c r="D109" s="98" t="s">
+      <c r="D109" s="100" t="s">
         <v>60</v>
       </c>
-      <c r="E109" s="99" t="s">
-        <v>141</v>
-      </c>
-      <c r="F109" s="99" t="s">
+      <c r="E109" s="101" t="s">
+        <v>141</v>
+      </c>
+      <c r="F109" s="101" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A110" s="98" t="s">
+      <c r="A110" s="100" t="s">
         <v>233</v>
       </c>
-      <c r="B110" s="98" t="s">
+      <c r="B110" s="100" t="s">
         <v>29</v>
       </c>
-      <c r="C110" s="98" t="s">
+      <c r="C110" s="100" t="s">
         <v>298</v>
       </c>
-      <c r="D110" s="98" t="s">
+      <c r="D110" s="100" t="s">
         <v>39</v>
       </c>
-      <c r="E110" s="99" t="s">
-        <v>141</v>
-      </c>
-      <c r="F110" s="99" t="s">
+      <c r="E110" s="101" t="s">
+        <v>141</v>
+      </c>
+      <c r="F110" s="101" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A111" s="98" t="s">
+      <c r="A111" s="100" t="s">
         <v>233</v>
       </c>
-      <c r="B111" s="98" t="s">
+      <c r="B111" s="100" t="s">
         <v>29</v>
       </c>
-      <c r="C111" s="98" t="s">
+      <c r="C111" s="100" t="s">
         <v>288</v>
       </c>
-      <c r="D111" s="98" t="s">
+      <c r="D111" s="100" t="s">
         <v>152</v>
       </c>
-      <c r="E111" s="99" t="s">
-        <v>141</v>
-      </c>
-      <c r="F111" s="99" t="s">
+      <c r="E111" s="101" t="s">
+        <v>141</v>
+      </c>
+      <c r="F111" s="101" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A112" s="98" t="s">
+      <c r="A112" s="100" t="s">
         <v>233</v>
       </c>
-      <c r="B112" s="98" t="s">
+      <c r="B112" s="100" t="s">
         <v>29</v>
       </c>
-      <c r="C112" s="98" t="s">
+      <c r="C112" s="100" t="s">
         <v>289</v>
       </c>
-      <c r="D112" s="98" t="s">
+      <c r="D112" s="100" t="s">
         <v>151</v>
       </c>
-      <c r="E112" s="99" t="s">
-        <v>141</v>
-      </c>
-      <c r="F112" s="99" t="s">
+      <c r="E112" s="101" t="s">
+        <v>141</v>
+      </c>
+      <c r="F112" s="101" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A113" s="98" t="s">
+      <c r="A113" s="100" t="s">
         <v>233</v>
       </c>
-      <c r="B113" s="98" t="s">
+      <c r="B113" s="100" t="s">
         <v>29</v>
       </c>
-      <c r="C113" s="98" t="s">
+      <c r="C113" s="100" t="s">
         <v>291</v>
       </c>
-      <c r="D113" s="98" t="s">
+      <c r="D113" s="100" t="s">
         <v>35</v>
       </c>
-      <c r="E113" s="99" t="s">
-        <v>141</v>
-      </c>
-      <c r="F113" s="99" t="s">
+      <c r="E113" s="101" t="s">
+        <v>141</v>
+      </c>
+      <c r="F113" s="101" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A114" s="98" t="s">
+      <c r="A114" s="100" t="s">
         <v>233</v>
       </c>
-      <c r="B114" s="98" t="s">
+      <c r="B114" s="100" t="s">
         <v>29</v>
       </c>
-      <c r="C114" s="98" t="s">
+      <c r="C114" s="100" t="s">
         <v>290</v>
       </c>
-      <c r="D114" s="98" t="s">
+      <c r="D114" s="100" t="s">
         <v>34</v>
       </c>
-      <c r="E114" s="99" t="s">
-        <v>141</v>
-      </c>
-      <c r="F114" s="99" t="s">
+      <c r="E114" s="101" t="s">
+        <v>141</v>
+      </c>
+      <c r="F114" s="101" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A115" s="98" t="s">
+      <c r="A115" s="100" t="s">
         <v>233</v>
       </c>
-      <c r="B115" s="98" t="s">
+      <c r="B115" s="100" t="s">
         <v>29</v>
       </c>
-      <c r="C115" s="98" t="s">
+      <c r="C115" s="100" t="s">
         <v>297</v>
       </c>
-      <c r="D115" s="98" t="s">
+      <c r="D115" s="100" t="s">
         <v>33</v>
       </c>
-      <c r="E115" s="99" t="s">
-        <v>141</v>
-      </c>
-      <c r="F115" s="99" t="s">
+      <c r="E115" s="101" t="s">
+        <v>141</v>
+      </c>
+      <c r="F115" s="101" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A116" s="98" t="s">
+      <c r="A116" s="100" t="s">
         <v>233</v>
       </c>
-      <c r="B116" s="98" t="s">
+      <c r="B116" s="100" t="s">
         <v>29</v>
       </c>
-      <c r="C116" s="98" t="s">
+      <c r="C116" s="100" t="s">
         <v>296</v>
       </c>
-      <c r="D116" s="98" t="s">
+      <c r="D116" s="100" t="s">
         <v>32</v>
       </c>
-      <c r="E116" s="99" t="s">
-        <v>141</v>
-      </c>
-      <c r="F116" s="99" t="s">
+      <c r="E116" s="101" t="s">
+        <v>141</v>
+      </c>
+      <c r="F116" s="101" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A117" s="98" t="s">
+      <c r="A117" s="100" t="s">
         <v>233</v>
       </c>
-      <c r="B117" s="98" t="s">
+      <c r="B117" s="100" t="s">
         <v>29</v>
       </c>
-      <c r="C117" s="98" t="s">
+      <c r="C117" s="100" t="s">
         <v>295</v>
       </c>
-      <c r="D117" s="98" t="s">
+      <c r="D117" s="100" t="s">
         <v>31</v>
       </c>
-      <c r="E117" s="99" t="s">
-        <v>141</v>
-      </c>
-      <c r="F117" s="99" t="s">
+      <c r="E117" s="101" t="s">
+        <v>141</v>
+      </c>
+      <c r="F117" s="101" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A118" s="98" t="s">
+      <c r="A118" s="100" t="s">
         <v>233</v>
       </c>
-      <c r="B118" s="98" t="s">
+      <c r="B118" s="100" t="s">
         <v>29</v>
       </c>
-      <c r="C118" s="98" t="s">
+      <c r="C118" s="100" t="s">
         <v>294</v>
       </c>
-      <c r="D118" s="98" t="s">
+      <c r="D118" s="100" t="s">
         <v>144</v>
       </c>
-      <c r="E118" s="99" t="s">
-        <v>141</v>
-      </c>
-      <c r="F118" s="99" t="s">
+      <c r="E118" s="101" t="s">
+        <v>141</v>
+      </c>
+      <c r="F118" s="101" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A119" s="98" t="s">
+      <c r="A119" s="100" t="s">
         <v>233</v>
       </c>
-      <c r="B119" s="98" t="s">
+      <c r="B119" s="100" t="s">
         <v>29</v>
       </c>
-      <c r="C119" s="98" t="s">
+      <c r="C119" s="100" t="s">
         <v>292</v>
       </c>
-      <c r="D119" s="98" t="s">
+      <c r="D119" s="100" t="s">
         <v>153</v>
       </c>
-      <c r="E119" s="99" t="s">
-        <v>141</v>
-      </c>
-      <c r="F119" s="99" t="s">
+      <c r="E119" s="101" t="s">
+        <v>141</v>
+      </c>
+      <c r="F119" s="101" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A120" s="98" t="s">
+      <c r="A120" s="100" t="s">
         <v>233</v>
       </c>
-      <c r="B120" s="98" t="s">
+      <c r="B120" s="100" t="s">
         <v>29</v>
       </c>
-      <c r="C120" s="98" t="s">
+      <c r="C120" s="100" t="s">
         <v>293</v>
       </c>
-      <c r="D120" s="98" t="s">
+      <c r="D120" s="100" t="s">
         <v>40</v>
       </c>
-      <c r="E120" s="99" t="s">
-        <v>141</v>
-      </c>
-      <c r="F120" s="99" t="s">
+      <c r="E120" s="101" t="s">
+        <v>141</v>
+      </c>
+      <c r="F120" s="101" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A121" s="98" t="s">
+      <c r="A121" s="100" t="s">
         <v>233</v>
       </c>
-      <c r="B121" s="98" t="s">
+      <c r="B121" s="100" t="s">
         <v>29</v>
       </c>
-      <c r="C121" s="98" t="s">
+      <c r="C121" s="100" t="s">
         <v>299</v>
       </c>
-      <c r="D121" s="98" t="s">
+      <c r="D121" s="100" t="s">
         <v>38</v>
       </c>
-      <c r="E121" s="99" t="s">
-        <v>141</v>
-      </c>
-      <c r="F121" s="99" t="s">
+      <c r="E121" s="101" t="s">
+        <v>141</v>
+      </c>
+      <c r="F121" s="101" t="s">
         <v>141</v>
       </c>
     </row>

</xml_diff>